<commit_message>
Set density requirement to 70%
</commit_message>
<xml_diff>
--- a/output_low_density_straight_sort.xlsx
+++ b/output_low_density_straight_sort.xlsx
@@ -587,7 +587,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>927</v>
+        <v>720</v>
       </c>
     </row>
     <row r="12">
@@ -657,7 +657,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>707</v>
+        <v>500</v>
       </c>
     </row>
     <row r="17">
@@ -685,7 +685,7 @@
         <v>1</v>
       </c>
       <c r="D18" t="n">
-        <v>814</v>
+        <v>607</v>
       </c>
     </row>
     <row r="19">
@@ -741,7 +741,7 @@
         <v>1</v>
       </c>
       <c r="D22" t="n">
-        <v>1114</v>
+        <v>907</v>
       </c>
     </row>
     <row r="23">
@@ -769,7 +769,7 @@
         <v>1</v>
       </c>
       <c r="D24" t="n">
-        <v>607</v>
+        <v>400</v>
       </c>
     </row>
     <row r="25">
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="D27" t="n">
-        <v>755</v>
+        <v>550</v>
       </c>
     </row>
     <row r="28">
@@ -853,7 +853,7 @@
         <v>1</v>
       </c>
       <c r="D30" t="n">
-        <v>914</v>
+        <v>707</v>
       </c>
     </row>
     <row r="31">
@@ -909,7 +909,7 @@
         <v>1</v>
       </c>
       <c r="D34" t="n">
-        <v>685</v>
+        <v>480</v>
       </c>
     </row>
     <row r="35">
@@ -965,7 +965,7 @@
         <v>1</v>
       </c>
       <c r="D38" t="n">
-        <v>835</v>
+        <v>640</v>
       </c>
     </row>
     <row r="39">
@@ -1021,7 +1021,7 @@
         <v>1</v>
       </c>
       <c r="D42" t="n">
-        <v>855</v>
+        <v>650</v>
       </c>
     </row>
     <row r="43">
@@ -1035,7 +1035,7 @@
         <v>1</v>
       </c>
       <c r="D43" t="n">
-        <v>1121</v>
+        <v>914</v>
       </c>
     </row>
     <row r="44">
@@ -1049,7 +1049,7 @@
         <v>1</v>
       </c>
       <c r="D44" t="n">
-        <v>757</v>
+        <v>550</v>
       </c>
     </row>
     <row r="45">
@@ -1077,7 +1077,7 @@
         <v>1</v>
       </c>
       <c r="D46" t="n">
-        <v>1007</v>
+        <v>800</v>
       </c>
     </row>
     <row r="47">
@@ -1189,7 +1189,7 @@
         <v>1</v>
       </c>
       <c r="D54" t="n">
-        <v>505</v>
+        <v>355</v>
       </c>
     </row>
     <row r="55">
@@ -1203,7 +1203,7 @@
         <v>1</v>
       </c>
       <c r="D55" t="n">
-        <v>914</v>
+        <v>707</v>
       </c>
     </row>
     <row r="56">
@@ -1287,7 +1287,7 @@
         <v>1</v>
       </c>
       <c r="D61" t="n">
-        <v>1201</v>
+        <v>994</v>
       </c>
     </row>
     <row r="62">
@@ -1301,7 +1301,7 @@
         <v>1</v>
       </c>
       <c r="D62" t="n">
-        <v>740</v>
+        <v>490</v>
       </c>
     </row>
     <row r="63">
@@ -1357,7 +1357,7 @@
         <v>1</v>
       </c>
       <c r="D66" t="n">
-        <v>994</v>
+        <v>787</v>
       </c>
     </row>
     <row r="67">
@@ -1371,7 +1371,7 @@
         <v>1</v>
       </c>
       <c r="D67" t="n">
-        <v>550</v>
+        <v>400</v>
       </c>
     </row>
     <row r="68">
@@ -1399,7 +1399,7 @@
         <v>1</v>
       </c>
       <c r="D69" t="n">
-        <v>1537</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="70">
@@ -1455,7 +1455,7 @@
         <v>1</v>
       </c>
       <c r="D73" t="n">
-        <v>984</v>
+        <v>777</v>
       </c>
     </row>
     <row r="74">
@@ -1469,7 +1469,7 @@
         <v>1</v>
       </c>
       <c r="D74" t="n">
-        <v>814</v>
+        <v>607</v>
       </c>
     </row>
     <row r="75">
@@ -1483,7 +1483,7 @@
         <v>1</v>
       </c>
       <c r="D75" t="n">
-        <v>857</v>
+        <v>500</v>
       </c>
     </row>
     <row r="76">
@@ -1693,7 +1693,7 @@
         <v>1</v>
       </c>
       <c r="D90" t="n">
-        <v>687</v>
+        <v>480</v>
       </c>
     </row>
     <row r="91">
@@ -1707,7 +1707,7 @@
         <v>1</v>
       </c>
       <c r="D91" t="n">
-        <v>1037</v>
+        <v>830</v>
       </c>
     </row>
     <row r="92">
@@ -1777,7 +1777,7 @@
         <v>1</v>
       </c>
       <c r="D96" t="n">
-        <v>550</v>
+        <v>400</v>
       </c>
     </row>
     <row r="97">
@@ -2127,7 +2127,7 @@
         <v>1</v>
       </c>
       <c r="D121" t="n">
-        <v>1064</v>
+        <v>857</v>
       </c>
     </row>
     <row r="122">
@@ -2309,7 +2309,7 @@
         <v>1</v>
       </c>
       <c r="D134" t="n">
-        <v>700</v>
+        <v>550</v>
       </c>
     </row>
     <row r="135">
@@ -2379,7 +2379,7 @@
         <v>1</v>
       </c>
       <c r="D139" t="n">
-        <v>990</v>
+        <v>650</v>
       </c>
     </row>
     <row r="140">
@@ -2407,7 +2407,7 @@
         <v>1</v>
       </c>
       <c r="D141" t="n">
-        <v>1801</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="142">
@@ -2435,7 +2435,7 @@
         <v>1</v>
       </c>
       <c r="D143" t="n">
-        <v>835</v>
+        <v>630</v>
       </c>
     </row>
     <row r="144">
@@ -2449,7 +2449,7 @@
         <v>1</v>
       </c>
       <c r="D144" t="n">
-        <v>1255</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="145">
@@ -2477,7 +2477,7 @@
         <v>1</v>
       </c>
       <c r="D146" t="n">
-        <v>1766</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="147">
@@ -2561,7 +2561,7 @@
         <v>1</v>
       </c>
       <c r="D152" t="n">
-        <v>1101</v>
+        <v>894</v>
       </c>
     </row>
     <row r="153">
@@ -2869,7 +2869,7 @@
         <v>1</v>
       </c>
       <c r="D174" t="n">
-        <v>920</v>
+        <v>580</v>
       </c>
     </row>
     <row r="175">
@@ -2911,7 +2911,7 @@
         <v>1</v>
       </c>
       <c r="D177" t="n">
-        <v>817</v>
+        <v>490</v>
       </c>
     </row>
     <row r="178">
@@ -2939,7 +2939,7 @@
         <v>1</v>
       </c>
       <c r="D179" t="n">
-        <v>814</v>
+        <v>607</v>
       </c>
     </row>
     <row r="180">
@@ -3037,7 +3037,7 @@
         <v>1</v>
       </c>
       <c r="D186" t="n">
-        <v>984</v>
+        <v>777</v>
       </c>
     </row>
     <row r="187">
@@ -3093,7 +3093,7 @@
         <v>1</v>
       </c>
       <c r="D190" t="n">
-        <v>847</v>
+        <v>697</v>
       </c>
     </row>
     <row r="191">
@@ -3163,7 +3163,7 @@
         <v>1</v>
       </c>
       <c r="D195" t="n">
-        <v>1164</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="196">
@@ -3233,7 +3233,7 @@
         <v>1</v>
       </c>
       <c r="D200" t="n">
-        <v>1315</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="201">
@@ -3275,7 +3275,7 @@
         <v>1</v>
       </c>
       <c r="D203" t="n">
-        <v>507</v>
+        <v>357</v>
       </c>
     </row>
     <row r="204">
@@ -3387,7 +3387,7 @@
         <v>1</v>
       </c>
       <c r="D211" t="n">
-        <v>1164</v>
+        <v>914</v>
       </c>
     </row>
     <row r="212">
@@ -3541,7 +3541,7 @@
         <v>1</v>
       </c>
       <c r="D222" t="n">
-        <v>607</v>
+        <v>400</v>
       </c>
     </row>
     <row r="223">
@@ -3597,7 +3597,7 @@
         <v>1</v>
       </c>
       <c r="D226" t="n">
-        <v>1464</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="227">
@@ -3681,7 +3681,7 @@
         <v>1</v>
       </c>
       <c r="D232" t="n">
-        <v>697</v>
+        <v>490</v>
       </c>
     </row>
     <row r="233">
@@ -3709,7 +3709,7 @@
         <v>1</v>
       </c>
       <c r="D234" t="n">
-        <v>705</v>
+        <v>500</v>
       </c>
     </row>
     <row r="235">
@@ -3751,7 +3751,7 @@
         <v>1</v>
       </c>
       <c r="D237" t="n">
-        <v>1478</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="238">
@@ -3779,7 +3779,7 @@
         <v>1</v>
       </c>
       <c r="D239" t="n">
-        <v>640</v>
+        <v>490</v>
       </c>
     </row>
     <row r="240">
@@ -3891,7 +3891,7 @@
         <v>1</v>
       </c>
       <c r="D247" t="n">
-        <v>847</v>
+        <v>640</v>
       </c>
     </row>
     <row r="248">
@@ -3905,7 +3905,7 @@
         <v>1</v>
       </c>
       <c r="D248" t="n">
-        <v>936</v>
+        <v>729</v>
       </c>
     </row>
     <row r="249">
@@ -3947,7 +3947,7 @@
         <v>1</v>
       </c>
       <c r="D251" t="n">
-        <v>550</v>
+        <v>400</v>
       </c>
     </row>
     <row r="252">
@@ -3961,7 +3961,7 @@
         <v>1</v>
       </c>
       <c r="D252" t="n">
-        <v>800</v>
+        <v>650</v>
       </c>
     </row>
     <row r="253">
@@ -3989,7 +3989,7 @@
         <v>1</v>
       </c>
       <c r="D254" t="n">
-        <v>605</v>
+        <v>400</v>
       </c>
     </row>
     <row r="255">
@@ -4129,7 +4129,7 @@
         <v>1</v>
       </c>
       <c r="D264" t="n">
-        <v>1329</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="265">
@@ -4227,7 +4227,7 @@
         <v>1</v>
       </c>
       <c r="D271" t="n">
-        <v>700</v>
+        <v>550</v>
       </c>
     </row>
     <row r="272">
@@ -4325,7 +4325,7 @@
         <v>1</v>
       </c>
       <c r="D278" t="n">
-        <v>640</v>
+        <v>490</v>
       </c>
     </row>
     <row r="279">
@@ -4381,7 +4381,7 @@
         <v>1</v>
       </c>
       <c r="D282" t="n">
-        <v>757</v>
+        <v>550</v>
       </c>
     </row>
     <row r="283">
@@ -4829,7 +4829,7 @@
         <v>1</v>
       </c>
       <c r="D314" t="n">
-        <v>707</v>
+        <v>500</v>
       </c>
     </row>
     <row r="315">
@@ -5179,7 +5179,7 @@
         <v>1</v>
       </c>
       <c r="D339" t="n">
-        <v>707</v>
+        <v>500</v>
       </c>
     </row>
     <row r="340">
@@ -5221,7 +5221,7 @@
         <v>1</v>
       </c>
       <c r="D342" t="n">
-        <v>707</v>
+        <v>500</v>
       </c>
     </row>
     <row r="343">
@@ -5515,7 +5515,7 @@
         <v>1</v>
       </c>
       <c r="D363" t="n">
-        <v>757</v>
+        <v>550</v>
       </c>
     </row>
     <row r="364">
@@ -5585,7 +5585,7 @@
         <v>1</v>
       </c>
       <c r="D368" t="n">
-        <v>707</v>
+        <v>500</v>
       </c>
     </row>
     <row r="369">
@@ -5669,7 +5669,7 @@
         <v>1</v>
       </c>
       <c r="D374" t="n">
-        <v>707</v>
+        <v>500</v>
       </c>
     </row>
     <row r="375">
@@ -5683,7 +5683,7 @@
         <v>1</v>
       </c>
       <c r="D375" t="n">
-        <v>904</v>
+        <v>697</v>
       </c>
     </row>
     <row r="376">
@@ -5711,7 +5711,7 @@
         <v>1</v>
       </c>
       <c r="D377" t="n">
-        <v>984</v>
+        <v>777</v>
       </c>
     </row>
     <row r="378">
@@ -5767,7 +5767,7 @@
         <v>1</v>
       </c>
       <c r="D381" t="n">
-        <v>707</v>
+        <v>500</v>
       </c>
     </row>
     <row r="382">
@@ -5795,7 +5795,7 @@
         <v>1</v>
       </c>
       <c r="D383" t="n">
-        <v>673</v>
+        <v>523</v>
       </c>
     </row>
     <row r="384">
@@ -6089,7 +6089,7 @@
         <v>1</v>
       </c>
       <c r="D404" t="n">
-        <v>787</v>
+        <v>580</v>
       </c>
     </row>
     <row r="405">
@@ -6173,7 +6173,7 @@
         <v>1</v>
       </c>
       <c r="D410" t="n">
-        <v>607</v>
+        <v>400</v>
       </c>
     </row>
     <row r="411">
@@ -6397,7 +6397,7 @@
         <v>1</v>
       </c>
       <c r="D426" t="n">
-        <v>840</v>
+        <v>500</v>
       </c>
     </row>
     <row r="427">
@@ -6495,7 +6495,7 @@
         <v>1</v>
       </c>
       <c r="D433" t="n">
-        <v>765</v>
+        <v>560</v>
       </c>
     </row>
     <row r="434">
@@ -6509,7 +6509,7 @@
         <v>1</v>
       </c>
       <c r="D434" t="n">
-        <v>707</v>
+        <v>500</v>
       </c>
     </row>
     <row r="435">
@@ -6621,7 +6621,7 @@
         <v>1</v>
       </c>
       <c r="D442" t="n">
-        <v>707</v>
+        <v>500</v>
       </c>
     </row>
     <row r="443">
@@ -6691,7 +6691,7 @@
         <v>1</v>
       </c>
       <c r="D447" t="n">
-        <v>904</v>
+        <v>697</v>
       </c>
     </row>
     <row r="448">
@@ -6733,7 +6733,7 @@
         <v>1</v>
       </c>
       <c r="D450" t="n">
-        <v>707</v>
+        <v>500</v>
       </c>
     </row>
     <row r="451">
@@ -6803,7 +6803,7 @@
         <v>1</v>
       </c>
       <c r="D455" t="n">
-        <v>1007</v>
+        <v>857</v>
       </c>
     </row>
     <row r="456">
@@ -6859,7 +6859,7 @@
         <v>1</v>
       </c>
       <c r="D459" t="n">
-        <v>777</v>
+        <v>570</v>
       </c>
     </row>
     <row r="460">
@@ -7083,7 +7083,7 @@
         <v>1</v>
       </c>
       <c r="D475" t="n">
-        <v>1121</v>
+        <v>914</v>
       </c>
     </row>
     <row r="476">
@@ -7111,7 +7111,7 @@
         <v>1</v>
       </c>
       <c r="D477" t="n">
-        <v>1618</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="478">
@@ -7139,7 +7139,7 @@
         <v>1</v>
       </c>
       <c r="D479" t="n">
-        <v>1201</v>
+        <v>994</v>
       </c>
     </row>
     <row r="480">
@@ -7153,7 +7153,7 @@
         <v>1</v>
       </c>
       <c r="D480" t="n">
-        <v>1121</v>
+        <v>914</v>
       </c>
     </row>
     <row r="481">
@@ -7167,7 +7167,7 @@
         <v>1</v>
       </c>
       <c r="D481" t="n">
-        <v>650</v>
+        <v>500</v>
       </c>
     </row>
     <row r="482">
@@ -7307,7 +7307,7 @@
         <v>1</v>
       </c>
       <c r="D491" t="n">
-        <v>992</v>
+        <v>787</v>
       </c>
     </row>
     <row r="492">
@@ -7321,7 +7321,7 @@
         <v>1</v>
       </c>
       <c r="D492" t="n">
-        <v>650</v>
+        <v>500</v>
       </c>
     </row>
     <row r="493">
@@ -7377,7 +7377,7 @@
         <v>1</v>
       </c>
       <c r="D496" t="n">
-        <v>914</v>
+        <v>707</v>
       </c>
     </row>
     <row r="497">
@@ -7405,7 +7405,7 @@
         <v>2</v>
       </c>
       <c r="D498" t="n">
-        <v>1234</v>
+        <v>984</v>
       </c>
     </row>
     <row r="499">
@@ -7461,7 +7461,7 @@
         <v>1</v>
       </c>
       <c r="D502" t="n">
-        <v>994</v>
+        <v>787</v>
       </c>
     </row>
     <row r="503">
@@ -7475,7 +7475,7 @@
         <v>1</v>
       </c>
       <c r="D503" t="n">
-        <v>1207</v>
+        <v>867</v>
       </c>
     </row>
     <row r="504">
@@ -7531,7 +7531,7 @@
         <v>1</v>
       </c>
       <c r="D507" t="n">
-        <v>707</v>
+        <v>500</v>
       </c>
     </row>
     <row r="508">
@@ -7587,7 +7587,7 @@
         <v>1</v>
       </c>
       <c r="D511" t="n">
-        <v>705</v>
+        <v>500</v>
       </c>
     </row>
     <row r="512">
@@ -7727,7 +7727,7 @@
         <v>1</v>
       </c>
       <c r="D521" t="n">
-        <v>785</v>
+        <v>580</v>
       </c>
     </row>
     <row r="522">
@@ -7755,7 +7755,7 @@
         <v>1</v>
       </c>
       <c r="D523" t="n">
-        <v>1414</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="524">
@@ -7797,7 +7797,7 @@
         <v>1</v>
       </c>
       <c r="D526" t="n">
-        <v>787</v>
+        <v>580</v>
       </c>
     </row>
     <row r="527">
@@ -7811,7 +7811,7 @@
         <v>1</v>
       </c>
       <c r="D527" t="n">
-        <v>992</v>
+        <v>787</v>
       </c>
     </row>
     <row r="528">
@@ -7909,7 +7909,7 @@
         <v>2</v>
       </c>
       <c r="D534" t="n">
-        <v>1000</v>
+        <v>850</v>
       </c>
     </row>
     <row r="535">
@@ -7937,7 +7937,7 @@
         <v>1</v>
       </c>
       <c r="D536" t="n">
-        <v>1074</v>
+        <v>867</v>
       </c>
     </row>
     <row r="537">
@@ -7951,7 +7951,7 @@
         <v>1</v>
       </c>
       <c r="D537" t="n">
-        <v>1010</v>
+        <v>860</v>
       </c>
     </row>
     <row r="538">
@@ -7979,7 +7979,7 @@
         <v>1</v>
       </c>
       <c r="D539" t="n">
-        <v>994</v>
+        <v>787</v>
       </c>
     </row>
     <row r="540">
@@ -8007,7 +8007,7 @@
         <v>1</v>
       </c>
       <c r="D541" t="n">
-        <v>785</v>
+        <v>580</v>
       </c>
     </row>
     <row r="542">
@@ -8245,7 +8245,7 @@
         <v>1</v>
       </c>
       <c r="D558" t="n">
-        <v>707</v>
+        <v>500</v>
       </c>
     </row>
     <row r="559">
@@ -8329,7 +8329,7 @@
         <v>1</v>
       </c>
       <c r="D564" t="n">
-        <v>650</v>
+        <v>500</v>
       </c>
     </row>
     <row r="565">
@@ -8385,7 +8385,7 @@
         <v>1</v>
       </c>
       <c r="D568" t="n">
-        <v>1271</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="569">
@@ -8399,7 +8399,7 @@
         <v>1</v>
       </c>
       <c r="D569" t="n">
-        <v>914</v>
+        <v>707</v>
       </c>
     </row>
     <row r="570">
@@ -8525,7 +8525,7 @@
         <v>1</v>
       </c>
       <c r="D578" t="n">
-        <v>787</v>
+        <v>580</v>
       </c>
     </row>
     <row r="579">
@@ -8539,7 +8539,7 @@
         <v>1</v>
       </c>
       <c r="D579" t="n">
-        <v>1064</v>
+        <v>857</v>
       </c>
     </row>
     <row r="580">
@@ -8581,7 +8581,7 @@
         <v>1</v>
       </c>
       <c r="D582" t="n">
-        <v>1421</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="583">
@@ -8595,7 +8595,7 @@
         <v>1</v>
       </c>
       <c r="D583" t="n">
-        <v>550</v>
+        <v>400</v>
       </c>
     </row>
     <row r="584">
@@ -8665,7 +8665,7 @@
         <v>2</v>
       </c>
       <c r="D588" t="n">
-        <v>1420</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="589">
@@ -8735,7 +8735,7 @@
         <v>1</v>
       </c>
       <c r="D593" t="n">
-        <v>1614</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="594">
@@ -8749,7 +8749,7 @@
         <v>1</v>
       </c>
       <c r="D594" t="n">
-        <v>994</v>
+        <v>787</v>
       </c>
     </row>
     <row r="595">
@@ -8791,7 +8791,7 @@
         <v>1</v>
       </c>
       <c r="D597" t="n">
-        <v>1520</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="598">
@@ -8805,7 +8805,7 @@
         <v>1</v>
       </c>
       <c r="D598" t="n">
-        <v>994</v>
+        <v>787</v>
       </c>
     </row>
     <row r="599">
@@ -8847,7 +8847,7 @@
         <v>1</v>
       </c>
       <c r="D601" t="n">
-        <v>697</v>
+        <v>490</v>
       </c>
     </row>
     <row r="602">
@@ -8889,7 +8889,7 @@
         <v>1</v>
       </c>
       <c r="D604" t="n">
-        <v>915</v>
+        <v>710</v>
       </c>
     </row>
     <row r="605">
@@ -9085,7 +9085,7 @@
         <v>1</v>
       </c>
       <c r="D618" t="n">
-        <v>1064</v>
+        <v>857</v>
       </c>
     </row>
     <row r="619">
@@ -9169,7 +9169,7 @@
         <v>1</v>
       </c>
       <c r="D624" t="n">
-        <v>840</v>
+        <v>500</v>
       </c>
     </row>
     <row r="625">
@@ -9477,7 +9477,7 @@
         <v>1</v>
       </c>
       <c r="D646" t="n">
-        <v>817</v>
+        <v>622</v>
       </c>
     </row>
     <row r="647">
@@ -9491,7 +9491,7 @@
         <v>1</v>
       </c>
       <c r="D647" t="n">
-        <v>1394</v>
+        <v>787</v>
       </c>
     </row>
     <row r="648">
@@ -9533,7 +9533,7 @@
         <v>2</v>
       </c>
       <c r="D650" t="n">
-        <v>964</v>
+        <v>607</v>
       </c>
     </row>
     <row r="651">
@@ -9603,7 +9603,7 @@
         <v>1</v>
       </c>
       <c r="D655" t="n">
-        <v>707</v>
+        <v>500</v>
       </c>
     </row>
     <row r="656">
@@ -9743,7 +9743,7 @@
         <v>1</v>
       </c>
       <c r="D665" t="n">
-        <v>914</v>
+        <v>707</v>
       </c>
     </row>
     <row r="666">
@@ -9799,7 +9799,7 @@
         <v>1</v>
       </c>
       <c r="D669" t="n">
-        <v>707</v>
+        <v>500</v>
       </c>
     </row>
     <row r="670">
@@ -10177,7 +10177,7 @@
         <v>1</v>
       </c>
       <c r="D696" t="n">
-        <v>914</v>
+        <v>707</v>
       </c>
     </row>
     <row r="697">
@@ -10247,7 +10247,7 @@
         <v>1</v>
       </c>
       <c r="D701" t="n">
-        <v>1047</v>
+        <v>707</v>
       </c>
     </row>
     <row r="702">
@@ -10415,7 +10415,7 @@
         <v>1</v>
       </c>
       <c r="D713" t="n">
-        <v>607</v>
+        <v>400</v>
       </c>
     </row>
     <row r="714">
@@ -10443,7 +10443,7 @@
         <v>1</v>
       </c>
       <c r="D715" t="n">
-        <v>894</v>
+        <v>687</v>
       </c>
     </row>
     <row r="716">
@@ -10499,7 +10499,7 @@
         <v>1</v>
       </c>
       <c r="D719" t="n">
-        <v>840</v>
+        <v>500</v>
       </c>
     </row>
     <row r="720">
@@ -10513,7 +10513,7 @@
         <v>1</v>
       </c>
       <c r="D720" t="n">
-        <v>707</v>
+        <v>500</v>
       </c>
     </row>
     <row r="721">
@@ -10569,7 +10569,7 @@
         <v>1</v>
       </c>
       <c r="D724" t="n">
-        <v>1054</v>
+        <v>697</v>
       </c>
     </row>
     <row r="725">
@@ -10625,7 +10625,7 @@
         <v>1</v>
       </c>
       <c r="D728" t="n">
-        <v>607</v>
+        <v>400</v>
       </c>
     </row>
     <row r="729">
@@ -10695,7 +10695,7 @@
         <v>1</v>
       </c>
       <c r="D733" t="n">
-        <v>800</v>
+        <v>650</v>
       </c>
     </row>
     <row r="734">
@@ -10793,7 +10793,7 @@
         <v>1</v>
       </c>
       <c r="D740" t="n">
-        <v>640</v>
+        <v>490</v>
       </c>
     </row>
     <row r="741">
@@ -10863,7 +10863,7 @@
         <v>1</v>
       </c>
       <c r="D745" t="n">
-        <v>730</v>
+        <v>580</v>
       </c>
     </row>
     <row r="746">
@@ -10891,7 +10891,7 @@
         <v>1</v>
       </c>
       <c r="D747" t="n">
-        <v>657</v>
+        <v>507</v>
       </c>
     </row>
     <row r="748">
@@ -11143,7 +11143,7 @@
         <v>1</v>
       </c>
       <c r="D765" t="n">
-        <v>1186</v>
+        <v>829</v>
       </c>
     </row>
     <row r="766">
@@ -11157,7 +11157,7 @@
         <v>1</v>
       </c>
       <c r="D766" t="n">
-        <v>1037</v>
+        <v>830</v>
       </c>
     </row>
     <row r="767">
@@ -11171,7 +11171,7 @@
         <v>2</v>
       </c>
       <c r="D767" t="n">
-        <v>845</v>
+        <v>640</v>
       </c>
     </row>
     <row r="768">
@@ -11213,7 +11213,7 @@
         <v>1</v>
       </c>
       <c r="D770" t="n">
-        <v>984</v>
+        <v>777</v>
       </c>
     </row>
     <row r="771">
@@ -11283,7 +11283,7 @@
         <v>2</v>
       </c>
       <c r="D775" t="n">
-        <v>1530</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="776">
@@ -11367,7 +11367,7 @@
         <v>1</v>
       </c>
       <c r="D781" t="n">
-        <v>787</v>
+        <v>580</v>
       </c>
     </row>
     <row r="782">
@@ -11395,7 +11395,7 @@
         <v>1</v>
       </c>
       <c r="D783" t="n">
-        <v>550</v>
+        <v>400</v>
       </c>
     </row>
     <row r="784">
@@ -11717,7 +11717,7 @@
         <v>1</v>
       </c>
       <c r="D806" t="n">
-        <v>1214</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="807">
@@ -11731,7 +11731,7 @@
         <v>1</v>
       </c>
       <c r="D807" t="n">
-        <v>1121</v>
+        <v>914</v>
       </c>
     </row>
     <row r="808">
@@ -11997,7 +11997,7 @@
         <v>1</v>
       </c>
       <c r="D826" t="n">
-        <v>914</v>
+        <v>707</v>
       </c>
     </row>
     <row r="827">
@@ -12179,7 +12179,7 @@
         <v>1</v>
       </c>
       <c r="D839" t="n">
-        <v>777</v>
+        <v>570</v>
       </c>
     </row>
     <row r="840">
@@ -12291,7 +12291,7 @@
         <v>1</v>
       </c>
       <c r="D847" t="n">
-        <v>1210</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="848">
@@ -12333,7 +12333,7 @@
         <v>1</v>
       </c>
       <c r="D850" t="n">
-        <v>1117</v>
+        <v>867</v>
       </c>
     </row>
     <row r="851">
@@ -12403,7 +12403,7 @@
         <v>1</v>
       </c>
       <c r="D855" t="n">
-        <v>857</v>
+        <v>500</v>
       </c>
     </row>
     <row r="856">
@@ -12529,7 +12529,7 @@
         <v>1</v>
       </c>
       <c r="D864" t="n">
-        <v>650</v>
+        <v>500</v>
       </c>
     </row>
     <row r="865">
@@ -12543,7 +12543,7 @@
         <v>1</v>
       </c>
       <c r="D865" t="n">
-        <v>550</v>
+        <v>400</v>
       </c>
     </row>
     <row r="866">
@@ -12557,7 +12557,7 @@
         <v>1</v>
       </c>
       <c r="D866" t="n">
-        <v>1378</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="867">
@@ -12641,7 +12641,7 @@
         <v>1</v>
       </c>
       <c r="D872" t="n">
-        <v>1064</v>
+        <v>857</v>
       </c>
     </row>
     <row r="873">
@@ -12683,7 +12683,7 @@
         <v>1</v>
       </c>
       <c r="D875" t="n">
-        <v>894</v>
+        <v>687</v>
       </c>
     </row>
     <row r="876">
@@ -12781,7 +12781,7 @@
         <v>1</v>
       </c>
       <c r="D882" t="n">
-        <v>1654</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="883">
@@ -12809,7 +12809,7 @@
         <v>1</v>
       </c>
       <c r="D884" t="n">
-        <v>914</v>
+        <v>707</v>
       </c>
     </row>
     <row r="885">
@@ -12823,7 +12823,7 @@
         <v>1</v>
       </c>
       <c r="D885" t="n">
-        <v>700</v>
+        <v>550</v>
       </c>
     </row>
     <row r="886">
@@ -12865,7 +12865,7 @@
         <v>1</v>
       </c>
       <c r="D888" t="n">
-        <v>1054</v>
+        <v>904</v>
       </c>
     </row>
     <row r="889">
@@ -12893,7 +12893,7 @@
         <v>1</v>
       </c>
       <c r="D890" t="n">
-        <v>2068</v>
+        <v>1863</v>
       </c>
     </row>
     <row r="891">
@@ -12935,7 +12935,7 @@
         <v>1</v>
       </c>
       <c r="D893" t="n">
-        <v>650</v>
+        <v>500</v>
       </c>
     </row>
     <row r="894">
@@ -13019,7 +13019,7 @@
         <v>1</v>
       </c>
       <c r="D899" t="n">
-        <v>775</v>
+        <v>570</v>
       </c>
     </row>
     <row r="900">
@@ -13131,7 +13131,7 @@
         <v>1</v>
       </c>
       <c r="D907" t="n">
-        <v>1164</v>
+        <v>914</v>
       </c>
     </row>
     <row r="908">
@@ -13173,7 +13173,7 @@
         <v>1</v>
       </c>
       <c r="D910" t="n">
-        <v>914</v>
+        <v>707</v>
       </c>
     </row>
     <row r="911">
@@ -13271,7 +13271,7 @@
         <v>1</v>
       </c>
       <c r="D917" t="n">
-        <v>1408</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="918">
@@ -13313,7 +13313,7 @@
         <v>1</v>
       </c>
       <c r="D920" t="n">
-        <v>1214</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="921">
@@ -13411,7 +13411,7 @@
         <v>1</v>
       </c>
       <c r="D927" t="n">
-        <v>787</v>
+        <v>580</v>
       </c>
     </row>
     <row r="928">
@@ -13439,7 +13439,7 @@
         <v>1</v>
       </c>
       <c r="D929" t="n">
-        <v>957</v>
+        <v>707</v>
       </c>
     </row>
     <row r="930">
@@ -13677,7 +13677,7 @@
         <v>1</v>
       </c>
       <c r="D946" t="n">
-        <v>550</v>
+        <v>400</v>
       </c>
     </row>
     <row r="947">
@@ -13733,7 +13733,7 @@
         <v>1</v>
       </c>
       <c r="D950" t="n">
-        <v>904</v>
+        <v>697</v>
       </c>
     </row>
     <row r="951">
@@ -13747,7 +13747,7 @@
         <v>1</v>
       </c>
       <c r="D951" t="n">
-        <v>650</v>
+        <v>500</v>
       </c>
     </row>
     <row r="952">
@@ -13789,7 +13789,7 @@
         <v>1</v>
       </c>
       <c r="D954" t="n">
-        <v>1155</v>
+        <v>950</v>
       </c>
     </row>
     <row r="955">
@@ -13803,7 +13803,7 @@
         <v>1</v>
       </c>
       <c r="D955" t="n">
-        <v>785</v>
+        <v>580</v>
       </c>
     </row>
     <row r="956">
@@ -13817,7 +13817,7 @@
         <v>1</v>
       </c>
       <c r="D956" t="n">
-        <v>1074</v>
+        <v>867</v>
       </c>
     </row>
     <row r="957">
@@ -13929,7 +13929,7 @@
         <v>1</v>
       </c>
       <c r="D964" t="n">
-        <v>914</v>
+        <v>707</v>
       </c>
     </row>
     <row r="965">
@@ -13985,7 +13985,7 @@
         <v>1</v>
       </c>
       <c r="D968" t="n">
-        <v>972</v>
+        <v>765</v>
       </c>
     </row>
     <row r="969">
@@ -13999,7 +13999,7 @@
         <v>1</v>
       </c>
       <c r="D969" t="n">
-        <v>865</v>
+        <v>660</v>
       </c>
     </row>
     <row r="970">
@@ -14209,7 +14209,7 @@
         <v>1</v>
       </c>
       <c r="D984" t="n">
-        <v>787</v>
+        <v>580</v>
       </c>
     </row>
     <row r="985">
@@ -14335,7 +14335,7 @@
         <v>1</v>
       </c>
       <c r="D993" t="n">
-        <v>827</v>
+        <v>705</v>
       </c>
     </row>
     <row r="994">
@@ -14391,7 +14391,7 @@
         <v>1</v>
       </c>
       <c r="D997" t="n">
-        <v>810</v>
+        <v>660</v>
       </c>
     </row>
     <row r="998">
@@ -14671,7 +14671,7 @@
         <v>1</v>
       </c>
       <c r="D1017" t="n">
-        <v>1228</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="1018">
@@ -14783,7 +14783,7 @@
         <v>1</v>
       </c>
       <c r="D1025" t="n">
-        <v>857</v>
+        <v>650</v>
       </c>
     </row>
     <row r="1026">
@@ -14811,7 +14811,7 @@
         <v>1</v>
       </c>
       <c r="D1027" t="n">
-        <v>994</v>
+        <v>787</v>
       </c>
     </row>
     <row r="1028">
@@ -14853,7 +14853,7 @@
         <v>1</v>
       </c>
       <c r="D1030" t="n">
-        <v>1064</v>
+        <v>857</v>
       </c>
     </row>
     <row r="1031">
@@ -14909,7 +14909,7 @@
         <v>1</v>
       </c>
       <c r="D1034" t="n">
-        <v>914</v>
+        <v>957</v>
       </c>
     </row>
     <row r="1035">
@@ -14937,7 +14937,7 @@
         <v>2</v>
       </c>
       <c r="D1036" t="n">
-        <v>1090</v>
+        <v>840</v>
       </c>
     </row>
     <row r="1037">
@@ -15245,7 +15245,7 @@
         <v>1</v>
       </c>
       <c r="D1058" t="n">
-        <v>1074</v>
+        <v>867</v>
       </c>
     </row>
     <row r="1059">
@@ -15329,7 +15329,7 @@
         <v>1</v>
       </c>
       <c r="D1064" t="n">
-        <v>1254</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="1065">
@@ -15525,7 +15525,7 @@
         <v>1</v>
       </c>
       <c r="D1078" t="n">
-        <v>1254</v>
+        <v>914</v>
       </c>
     </row>
     <row r="1079">
@@ -15693,7 +15693,7 @@
         <v>1</v>
       </c>
       <c r="D1090" t="n">
-        <v>1527</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="1091">
@@ -15777,7 +15777,7 @@
         <v>1</v>
       </c>
       <c r="D1096" t="n">
-        <v>650</v>
+        <v>500</v>
       </c>
     </row>
     <row r="1097">
@@ -15791,7 +15791,7 @@
         <v>1</v>
       </c>
       <c r="D1097" t="n">
-        <v>1742</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="1098">
@@ -15819,7 +15819,7 @@
         <v>1</v>
       </c>
       <c r="D1099" t="n">
-        <v>1344</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="1100">
@@ -15861,7 +15861,7 @@
         <v>1</v>
       </c>
       <c r="D1102" t="n">
-        <v>1202</v>
+        <v>857</v>
       </c>
     </row>
     <row r="1103">
@@ -15917,7 +15917,7 @@
         <v>1</v>
       </c>
       <c r="D1106" t="n">
-        <v>787</v>
+        <v>580</v>
       </c>
     </row>
     <row r="1107">
@@ -16001,7 +16001,7 @@
         <v>1</v>
       </c>
       <c r="D1112" t="n">
-        <v>914</v>
+        <v>707</v>
       </c>
     </row>
     <row r="1113">
@@ -16141,7 +16141,7 @@
         <v>1</v>
       </c>
       <c r="D1122" t="n">
-        <v>707</v>
+        <v>500</v>
       </c>
     </row>
     <row r="1123">
@@ -16183,7 +16183,7 @@
         <v>1</v>
       </c>
       <c r="D1125" t="n">
-        <v>857</v>
+        <v>650</v>
       </c>
     </row>
     <row r="1126">
@@ -16225,7 +16225,7 @@
         <v>2</v>
       </c>
       <c r="D1128" t="n">
-        <v>1257</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="1129">
@@ -16253,7 +16253,7 @@
         <v>2</v>
       </c>
       <c r="D1130" t="n">
-        <v>705</v>
+        <v>500</v>
       </c>
     </row>
     <row r="1131">
@@ -16337,7 +16337,7 @@
         <v>1</v>
       </c>
       <c r="D1136" t="n">
-        <v>1074</v>
+        <v>867</v>
       </c>
     </row>
     <row r="1137">
@@ -16365,7 +16365,7 @@
         <v>1</v>
       </c>
       <c r="D1138" t="n">
-        <v>1000</v>
+        <v>660</v>
       </c>
     </row>
     <row r="1139">
@@ -16421,7 +16421,7 @@
         <v>2</v>
       </c>
       <c r="D1142" t="n">
-        <v>840</v>
+        <v>500</v>
       </c>
     </row>
     <row r="1143">
@@ -16505,7 +16505,7 @@
         <v>1</v>
       </c>
       <c r="D1148" t="n">
-        <v>1527</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="1149">
@@ -16519,7 +16519,7 @@
         <v>2</v>
       </c>
       <c r="D1149" t="n">
-        <v>990</v>
+        <v>650</v>
       </c>
     </row>
     <row r="1150">
@@ -16589,7 +16589,7 @@
         <v>1</v>
       </c>
       <c r="D1154" t="n">
-        <v>1064</v>
+        <v>857</v>
       </c>
     </row>
     <row r="1155">
@@ -16659,7 +16659,7 @@
         <v>1</v>
       </c>
       <c r="D1159" t="n">
-        <v>814</v>
+        <v>607</v>
       </c>
     </row>
     <row r="1160">
@@ -16701,7 +16701,7 @@
         <v>1</v>
       </c>
       <c r="D1162" t="n">
-        <v>650</v>
+        <v>500</v>
       </c>
     </row>
     <row r="1163">
@@ -16883,7 +16883,7 @@
         <v>1</v>
       </c>
       <c r="D1175" t="n">
-        <v>962</v>
+        <v>622</v>
       </c>
     </row>
     <row r="1176">
@@ -16953,7 +16953,7 @@
         <v>1</v>
       </c>
       <c r="D1180" t="n">
-        <v>772</v>
+        <v>622</v>
       </c>
     </row>
     <row r="1181">
@@ -16995,7 +16995,7 @@
         <v>1</v>
       </c>
       <c r="D1183" t="n">
-        <v>994</v>
+        <v>787</v>
       </c>
     </row>
     <row r="1184">
@@ -17009,7 +17009,7 @@
         <v>1</v>
       </c>
       <c r="D1184" t="n">
-        <v>730</v>
+        <v>580</v>
       </c>
     </row>
     <row r="1185">
@@ -17149,7 +17149,7 @@
         <v>1</v>
       </c>
       <c r="D1194" t="n">
-        <v>700</v>
+        <v>550</v>
       </c>
     </row>
     <row r="1195">
@@ -17177,7 +17177,7 @@
         <v>1</v>
       </c>
       <c r="D1196" t="n">
-        <v>1026</v>
+        <v>819</v>
       </c>
     </row>
     <row r="1197">
@@ -17401,7 +17401,7 @@
         <v>1</v>
       </c>
       <c r="D1212" t="n">
-        <v>994</v>
+        <v>787</v>
       </c>
     </row>
     <row r="1213">
@@ -17443,7 +17443,7 @@
         <v>1</v>
       </c>
       <c r="D1215" t="n">
-        <v>904</v>
+        <v>697</v>
       </c>
     </row>
     <row r="1216">
@@ -17485,7 +17485,7 @@
         <v>1</v>
       </c>
       <c r="D1218" t="n">
-        <v>707</v>
+        <v>500</v>
       </c>
     </row>
     <row r="1219">
@@ -17695,7 +17695,7 @@
         <v>1</v>
       </c>
       <c r="D1233" t="n">
-        <v>955</v>
+        <v>805</v>
       </c>
     </row>
     <row r="1234">
@@ -17849,7 +17849,7 @@
         <v>1</v>
       </c>
       <c r="D1244" t="n">
-        <v>1205</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="1245">
@@ -17877,7 +17877,7 @@
         <v>1</v>
       </c>
       <c r="D1246" t="n">
-        <v>1054</v>
+        <v>847</v>
       </c>
     </row>
     <row r="1247">
@@ -17905,7 +17905,7 @@
         <v>1</v>
       </c>
       <c r="D1248" t="n">
-        <v>750</v>
+        <v>500</v>
       </c>
     </row>
     <row r="1249">
@@ -17919,7 +17919,7 @@
         <v>1</v>
       </c>
       <c r="D1249" t="n">
-        <v>994</v>
+        <v>787</v>
       </c>
     </row>
     <row r="1250">
@@ -17933,7 +17933,7 @@
         <v>1</v>
       </c>
       <c r="D1250" t="n">
-        <v>757</v>
+        <v>400</v>
       </c>
     </row>
     <row r="1251">
@@ -18031,7 +18031,7 @@
         <v>1</v>
       </c>
       <c r="D1257" t="n">
-        <v>1210</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="1258">
@@ -18115,7 +18115,7 @@
         <v>1</v>
       </c>
       <c r="D1263" t="n">
-        <v>1535</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="1264">
@@ -18129,7 +18129,7 @@
         <v>1</v>
       </c>
       <c r="D1264" t="n">
-        <v>787</v>
+        <v>580</v>
       </c>
     </row>
     <row r="1265">
@@ -18143,7 +18143,7 @@
         <v>1</v>
       </c>
       <c r="D1265" t="n">
-        <v>787</v>
+        <v>580</v>
       </c>
     </row>
     <row r="1266">
@@ -18185,7 +18185,7 @@
         <v>1</v>
       </c>
       <c r="D1268" t="n">
-        <v>805</v>
+        <v>655</v>
       </c>
     </row>
     <row r="1269">
@@ -18255,7 +18255,7 @@
         <v>2</v>
       </c>
       <c r="D1273" t="n">
-        <v>1818</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="1274">
@@ -18283,7 +18283,7 @@
         <v>1</v>
       </c>
       <c r="D1275" t="n">
-        <v>910</v>
+        <v>705</v>
       </c>
     </row>
     <row r="1276">
@@ -18311,7 +18311,7 @@
         <v>1</v>
       </c>
       <c r="D1277" t="n">
-        <v>777</v>
+        <v>570</v>
       </c>
     </row>
     <row r="1278">
@@ -18409,7 +18409,7 @@
         <v>1</v>
       </c>
       <c r="D1284" t="n">
-        <v>1387</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1285">
@@ -18549,7 +18549,7 @@
         <v>1</v>
       </c>
       <c r="D1294" t="n">
-        <v>1074</v>
+        <v>867</v>
       </c>
     </row>
     <row r="1295">
@@ -18577,7 +18577,7 @@
         <v>1</v>
       </c>
       <c r="D1296" t="n">
-        <v>787</v>
+        <v>580</v>
       </c>
     </row>
     <row r="1297">
@@ -18591,7 +18591,7 @@
         <v>1</v>
       </c>
       <c r="D1297" t="n">
-        <v>1121</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="1298">
@@ -18675,7 +18675,7 @@
         <v>1</v>
       </c>
       <c r="D1303" t="n">
-        <v>705</v>
+        <v>500</v>
       </c>
     </row>
     <row r="1304">
@@ -18745,7 +18745,7 @@
         <v>1</v>
       </c>
       <c r="D1308" t="n">
-        <v>1074</v>
+        <v>867</v>
       </c>
     </row>
     <row r="1309">
@@ -18773,7 +18773,7 @@
         <v>1</v>
       </c>
       <c r="D1310" t="n">
-        <v>814</v>
+        <v>607</v>
       </c>
     </row>
     <row r="1311">
@@ -18843,7 +18843,7 @@
         <v>1</v>
       </c>
       <c r="D1315" t="n">
-        <v>914</v>
+        <v>707</v>
       </c>
     </row>
     <row r="1316">

</xml_diff>